<commit_message>
feat(mail,queue): menambahkan antrian mailer
</commit_message>
<xml_diff>
--- a/public/books.xlsx
+++ b/public/books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Laravel\librarium.informatica\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E03CD66-0E8B-4B3D-A8D8-69CECA62FF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0182E8-45F0-4757-8925-16C0A6E39829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,6 +36,33 @@
     <t>Gramedia</t>
   </si>
   <si>
+    <t>Buku A</t>
+  </si>
+  <si>
+    <t>Buku B</t>
+  </si>
+  <si>
+    <t>Buku C</t>
+  </si>
+  <si>
+    <t>Author A</t>
+  </si>
+  <si>
+    <t>Author B</t>
+  </si>
+  <si>
+    <t>Author C</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Solo</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
     <t>title</t>
   </si>
   <si>
@@ -51,37 +78,10 @@
     <t>city</t>
   </si>
   <si>
-    <t>quantity</t>
+    <t>categorie_id</t>
   </si>
   <si>
     <t>bookshelf_id</t>
-  </si>
-  <si>
-    <t>Buku A</t>
-  </si>
-  <si>
-    <t>Buku B</t>
-  </si>
-  <si>
-    <t>Buku C</t>
-  </si>
-  <si>
-    <t>Author A</t>
-  </si>
-  <si>
-    <t>Author B</t>
-  </si>
-  <si>
-    <t>Author C</t>
-  </si>
-  <si>
-    <t>Bandung</t>
-  </si>
-  <si>
-    <t>Solo</t>
-  </si>
-  <si>
-    <t>Jakarta</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,33 +438,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1998</v>
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -484,10 +484,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1998</v>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>1998</v>
@@ -519,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>3</v>

</xml_diff>